<commit_message>
20210528 CRD20-083	To extract information from eHS(S) for analysis of dental service claim by VRs’ age groups and places of practices in all districts in 2009-2020 20210531 CRE20-023-48	COVID-19 – Phase 48 	1.	Enhance VSS (Non-clinic) to support outreach to other premises 20210531 CRE21-003	To update the subsidy of COVID-19 Vaccination for RVP VMOs 20210604 CRE21-004	To present the selected claim transactions in the Post Payment Check Reports (i.e. PPC0002 and PPC0003) in a randomised way 20210604 CRE21-005	To exclude claim transactions related to COVID-19 vaccine subsidies in PPC0002, PPC0003, eHS(S)U0002
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/PPC0002-Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/PPC0002-Template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2021\CRE21-005 (Exclude C19 in PPC0002,PPC0003 and U0002)\Front-end\ExcelGenerator\Template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="6075" windowWidth="15375" windowHeight="2070" tabRatio="679"/>
   </bookViews>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Description</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -87,22 +92,50 @@
   <si>
     <t xml:space="preserve">To enhance the eHS(S) to cope with elders holding HKIC with “C” or “U” code </t>
   </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To present the selected claim transactions in the Post Payment Check Reports (i.e. PPC0002 and PPC0003) in a randomised way</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRE21-004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRE21-005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To exclude claim transactions related to COVID-19 vaccine subsidies in PPC0002, PPC0003, eHS(S)U0002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021/06/04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="yyyy\/mm\/dd\ hh:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="yyyy\/mm\/dd"/>
-    <numFmt numFmtId="167" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
+    <numFmt numFmtId="177" formatCode="yyyy\/mm\/dd\ hh:mm:ss"/>
+    <numFmt numFmtId="178" formatCode="yyyy\/mm\/dd"/>
+    <numFmt numFmtId="179" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -170,7 +203,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -305,7 +338,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -701,7 +734,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -822,58 +855,58 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -885,7 +918,7 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -899,6 +932,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1009,7 +1045,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1044,7 +1080,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1257,14 +1293,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="66.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1272,7 +1308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1280,7 +1316,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1288,7 +1324,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1296,7 +1332,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1304,7 +1340,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1312,7 +1348,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1320,7 +1356,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1328,7 +1364,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1336,7 +1372,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1344,7 +1380,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1352,7 +1388,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1360,7 +1396,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75">
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1378,7 +1414,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="13" customWidth="1"/>
@@ -1404,11 +1440,11 @@
     <col min="26" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
     </row>
-    <row r="3" spans="1:25" s="18" customFormat="1">
+    <row r="3" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="23"/>
       <c r="D3" s="21"/>
       <c r="J3" s="51"/>
@@ -1428,7 +1464,7 @@
       <c r="X3" s="54"/>
       <c r="Y3" s="19"/>
     </row>
-    <row r="4" spans="1:25" s="18" customFormat="1">
+    <row r="4" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="23"/>
       <c r="D4" s="21"/>
       <c r="J4" s="51"/>
@@ -1448,7 +1484,7 @@
       <c r="X4" s="54"/>
       <c r="Y4" s="19"/>
     </row>
-    <row r="5" spans="1:25" s="18" customFormat="1">
+    <row r="5" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="23"/>
       <c r="D5" s="21"/>
       <c r="J5" s="51"/>
@@ -1468,7 +1504,7 @@
       <c r="X5" s="54"/>
       <c r="Y5" s="19"/>
     </row>
-    <row r="6" spans="1:25" s="18" customFormat="1">
+    <row r="6" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="21"/>
       <c r="J6" s="51"/>
       <c r="K6" s="19"/>
@@ -1487,7 +1523,7 @@
       <c r="X6" s="54"/>
       <c r="Y6" s="19"/>
     </row>
-    <row r="7" spans="1:25" s="18" customFormat="1">
+    <row r="7" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="D7" s="21"/>
       <c r="F7" s="19"/>
@@ -1508,7 +1544,7 @@
       <c r="X7" s="54"/>
       <c r="Y7" s="19"/>
     </row>
-    <row r="8" spans="1:25" s="18" customFormat="1">
+    <row r="8" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="22"/>
@@ -1530,7 +1566,7 @@
       <c r="X8" s="54"/>
       <c r="Y8" s="19"/>
     </row>
-    <row r="9" spans="1:25" s="18" customFormat="1">
+    <row r="9" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="22"/>
@@ -1552,7 +1588,7 @@
       <c r="X9" s="54"/>
       <c r="Y9" s="19"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="18"/>
       <c r="C10" s="26"/>
@@ -1574,7 +1610,7 @@
       <c r="X10" s="55"/>
       <c r="Y10" s="26"/>
     </row>
-    <row r="11" spans="1:25" s="10" customFormat="1">
+    <row r="11" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="D11" s="33"/>
@@ -1597,7 +1633,7 @@
       <c r="X11" s="56"/>
       <c r="Y11" s="16"/>
     </row>
-    <row r="12" spans="1:25" s="30" customFormat="1">
+    <row r="12" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="34"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -1621,7 +1657,7 @@
       <c r="X12" s="57"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="1:25" s="30" customFormat="1">
+    <row r="13" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="34"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -1642,7 +1678,7 @@
       <c r="X13" s="57"/>
       <c r="Y13" s="15"/>
     </row>
-    <row r="14" spans="1:25" s="30" customFormat="1">
+    <row r="14" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="34"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -1663,7 +1699,7 @@
       <c r="X14" s="57"/>
       <c r="Y14" s="15"/>
     </row>
-    <row r="15" spans="1:25" s="30" customFormat="1">
+    <row r="15" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="34"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -1684,7 +1720,7 @@
       <c r="X15" s="57"/>
       <c r="Y15" s="15"/>
     </row>
-    <row r="16" spans="1:25" s="30" customFormat="1">
+    <row r="16" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="34"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1705,7 +1741,7 @@
       <c r="X16" s="57"/>
       <c r="Y16" s="15"/>
     </row>
-    <row r="17" spans="4:25" s="30" customFormat="1">
+    <row r="17" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="34"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -1726,7 +1762,7 @@
       <c r="X17" s="57"/>
       <c r="Y17" s="15"/>
     </row>
-    <row r="18" spans="4:25" s="30" customFormat="1">
+    <row r="18" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="34"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -1747,7 +1783,7 @@
       <c r="X18" s="57"/>
       <c r="Y18" s="15"/>
     </row>
-    <row r="19" spans="4:25" s="30" customFormat="1">
+    <row r="19" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="34"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -1768,7 +1804,7 @@
       <c r="X19" s="57"/>
       <c r="Y19" s="15"/>
     </row>
-    <row r="20" spans="4:25" s="30" customFormat="1">
+    <row r="20" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="34"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -1789,7 +1825,7 @@
       <c r="X20" s="57"/>
       <c r="Y20" s="15"/>
     </row>
-    <row r="21" spans="4:25" s="30" customFormat="1">
+    <row r="21" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="34"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -1810,7 +1846,7 @@
       <c r="X21" s="57"/>
       <c r="Y21" s="15"/>
     </row>
-    <row r="22" spans="4:25" s="30" customFormat="1">
+    <row r="22" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="34"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -1831,7 +1867,7 @@
       <c r="X22" s="57"/>
       <c r="Y22" s="15"/>
     </row>
-    <row r="23" spans="4:25" s="30" customFormat="1">
+    <row r="23" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="34"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -1852,7 +1888,7 @@
       <c r="X23" s="57"/>
       <c r="Y23" s="15"/>
     </row>
-    <row r="24" spans="4:25" s="30" customFormat="1">
+    <row r="24" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="34"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -1873,7 +1909,7 @@
       <c r="X24" s="57"/>
       <c r="Y24" s="15"/>
     </row>
-    <row r="25" spans="4:25" s="30" customFormat="1">
+    <row r="25" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="34"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -1894,7 +1930,7 @@
       <c r="X25" s="57"/>
       <c r="Y25" s="15"/>
     </row>
-    <row r="26" spans="4:25" s="30" customFormat="1">
+    <row r="26" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="34"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -1915,7 +1951,7 @@
       <c r="X26" s="57"/>
       <c r="Y26" s="15"/>
     </row>
-    <row r="27" spans="4:25" s="30" customFormat="1">
+    <row r="27" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="34"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -1936,7 +1972,7 @@
       <c r="X27" s="57"/>
       <c r="Y27" s="15"/>
     </row>
-    <row r="28" spans="4:25" s="30" customFormat="1">
+    <row r="28" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="34"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -1957,7 +1993,7 @@
       <c r="X28" s="57"/>
       <c r="Y28" s="15"/>
     </row>
-    <row r="29" spans="4:25" s="30" customFormat="1">
+    <row r="29" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="34"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -1978,7 +2014,7 @@
       <c r="X29" s="57"/>
       <c r="Y29" s="15"/>
     </row>
-    <row r="30" spans="4:25" s="30" customFormat="1">
+    <row r="30" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="34"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -2012,7 +2048,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="13" customWidth="1"/>
@@ -2038,11 +2074,11 @@
     <col min="26" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
     </row>
-    <row r="3" spans="1:25" s="18" customFormat="1">
+    <row r="3" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="23"/>
       <c r="D3" s="21"/>
       <c r="J3" s="51"/>
@@ -2062,7 +2098,7 @@
       <c r="X3" s="54"/>
       <c r="Y3" s="19"/>
     </row>
-    <row r="4" spans="1:25" s="18" customFormat="1">
+    <row r="4" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="23"/>
       <c r="D4" s="21"/>
       <c r="J4" s="51"/>
@@ -2082,7 +2118,7 @@
       <c r="X4" s="54"/>
       <c r="Y4" s="19"/>
     </row>
-    <row r="5" spans="1:25" s="18" customFormat="1">
+    <row r="5" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="23"/>
       <c r="D5" s="21"/>
       <c r="J5" s="51"/>
@@ -2102,7 +2138,7 @@
       <c r="X5" s="54"/>
       <c r="Y5" s="19"/>
     </row>
-    <row r="6" spans="1:25" s="18" customFormat="1">
+    <row r="6" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="21"/>
       <c r="J6" s="51"/>
       <c r="K6" s="19"/>
@@ -2121,7 +2157,7 @@
       <c r="X6" s="54"/>
       <c r="Y6" s="19"/>
     </row>
-    <row r="7" spans="1:25" s="18" customFormat="1">
+    <row r="7" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="D7" s="21"/>
       <c r="F7" s="19"/>
@@ -2142,7 +2178,7 @@
       <c r="X7" s="54"/>
       <c r="Y7" s="19"/>
     </row>
-    <row r="8" spans="1:25" s="18" customFormat="1">
+    <row r="8" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="22"/>
@@ -2164,7 +2200,7 @@
       <c r="X8" s="54"/>
       <c r="Y8" s="19"/>
     </row>
-    <row r="9" spans="1:25" s="18" customFormat="1">
+    <row r="9" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="22"/>
@@ -2186,7 +2222,7 @@
       <c r="X9" s="54"/>
       <c r="Y9" s="19"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="18"/>
       <c r="C10" s="26"/>
@@ -2208,7 +2244,7 @@
       <c r="X10" s="55"/>
       <c r="Y10" s="26"/>
     </row>
-    <row r="11" spans="1:25" s="10" customFormat="1">
+    <row r="11" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="D11" s="33"/>
@@ -2231,7 +2267,7 @@
       <c r="X11" s="56"/>
       <c r="Y11" s="16"/>
     </row>
-    <row r="12" spans="1:25" s="30" customFormat="1">
+    <row r="12" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="34"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -2255,7 +2291,7 @@
       <c r="X12" s="57"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="1:25" s="30" customFormat="1">
+    <row r="13" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="34"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -2276,7 +2312,7 @@
       <c r="X13" s="57"/>
       <c r="Y13" s="15"/>
     </row>
-    <row r="14" spans="1:25" s="30" customFormat="1">
+    <row r="14" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="34"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -2297,7 +2333,7 @@
       <c r="X14" s="57"/>
       <c r="Y14" s="15"/>
     </row>
-    <row r="15" spans="1:25" s="30" customFormat="1">
+    <row r="15" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="34"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -2318,7 +2354,7 @@
       <c r="X15" s="57"/>
       <c r="Y15" s="15"/>
     </row>
-    <row r="16" spans="1:25" s="30" customFormat="1">
+    <row r="16" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="34"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -2339,7 +2375,7 @@
       <c r="X16" s="57"/>
       <c r="Y16" s="15"/>
     </row>
-    <row r="17" spans="4:25" s="30" customFormat="1">
+    <row r="17" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="34"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -2360,7 +2396,7 @@
       <c r="X17" s="57"/>
       <c r="Y17" s="15"/>
     </row>
-    <row r="18" spans="4:25" s="30" customFormat="1">
+    <row r="18" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="34"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -2381,7 +2417,7 @@
       <c r="X18" s="57"/>
       <c r="Y18" s="15"/>
     </row>
-    <row r="19" spans="4:25" s="30" customFormat="1">
+    <row r="19" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="34"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -2402,7 +2438,7 @@
       <c r="X19" s="57"/>
       <c r="Y19" s="15"/>
     </row>
-    <row r="20" spans="4:25" s="30" customFormat="1">
+    <row r="20" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="34"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -2423,7 +2459,7 @@
       <c r="X20" s="57"/>
       <c r="Y20" s="15"/>
     </row>
-    <row r="21" spans="4:25" s="30" customFormat="1">
+    <row r="21" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="34"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -2444,7 +2480,7 @@
       <c r="X21" s="57"/>
       <c r="Y21" s="15"/>
     </row>
-    <row r="22" spans="4:25" s="30" customFormat="1">
+    <row r="22" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="34"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -2465,7 +2501,7 @@
       <c r="X22" s="57"/>
       <c r="Y22" s="15"/>
     </row>
-    <row r="23" spans="4:25" s="30" customFormat="1">
+    <row r="23" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="34"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -2486,7 +2522,7 @@
       <c r="X23" s="57"/>
       <c r="Y23" s="15"/>
     </row>
-    <row r="24" spans="4:25" s="30" customFormat="1">
+    <row r="24" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="34"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -2507,7 +2543,7 @@
       <c r="X24" s="57"/>
       <c r="Y24" s="15"/>
     </row>
-    <row r="25" spans="4:25" s="30" customFormat="1">
+    <row r="25" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="34"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -2528,7 +2564,7 @@
       <c r="X25" s="57"/>
       <c r="Y25" s="15"/>
     </row>
-    <row r="26" spans="4:25" s="30" customFormat="1">
+    <row r="26" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="34"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -2549,7 +2585,7 @@
       <c r="X26" s="57"/>
       <c r="Y26" s="15"/>
     </row>
-    <row r="27" spans="4:25" s="30" customFormat="1">
+    <row r="27" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="34"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -2570,7 +2606,7 @@
       <c r="X27" s="57"/>
       <c r="Y27" s="15"/>
     </row>
-    <row r="28" spans="4:25" s="30" customFormat="1">
+    <row r="28" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="34"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -2591,7 +2627,7 @@
       <c r="X28" s="57"/>
       <c r="Y28" s="15"/>
     </row>
-    <row r="29" spans="4:25" s="30" customFormat="1">
+    <row r="29" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="34"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -2612,7 +2648,7 @@
       <c r="X29" s="57"/>
       <c r="Y29" s="15"/>
     </row>
-    <row r="30" spans="4:25" s="30" customFormat="1">
+    <row r="30" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="34"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -2646,7 +2682,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="13" customWidth="1"/>
@@ -2672,11 +2708,11 @@
     <col min="26" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
     </row>
-    <row r="3" spans="1:25" s="18" customFormat="1">
+    <row r="3" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="23"/>
       <c r="D3" s="21"/>
       <c r="J3" s="51"/>
@@ -2696,7 +2732,7 @@
       <c r="X3" s="54"/>
       <c r="Y3" s="19"/>
     </row>
-    <row r="4" spans="1:25" s="18" customFormat="1">
+    <row r="4" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="23"/>
       <c r="D4" s="21"/>
       <c r="J4" s="51"/>
@@ -2716,7 +2752,7 @@
       <c r="X4" s="54"/>
       <c r="Y4" s="19"/>
     </row>
-    <row r="5" spans="1:25" s="18" customFormat="1">
+    <row r="5" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="23"/>
       <c r="D5" s="21"/>
       <c r="J5" s="51"/>
@@ -2736,7 +2772,7 @@
       <c r="X5" s="54"/>
       <c r="Y5" s="19"/>
     </row>
-    <row r="6" spans="1:25" s="18" customFormat="1">
+    <row r="6" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="21"/>
       <c r="J6" s="51"/>
       <c r="K6" s="19"/>
@@ -2755,7 +2791,7 @@
       <c r="X6" s="54"/>
       <c r="Y6" s="19"/>
     </row>
-    <row r="7" spans="1:25" s="18" customFormat="1">
+    <row r="7" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="D7" s="21"/>
       <c r="F7" s="19"/>
@@ -2776,7 +2812,7 @@
       <c r="X7" s="54"/>
       <c r="Y7" s="19"/>
     </row>
-    <row r="8" spans="1:25" s="18" customFormat="1">
+    <row r="8" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="22"/>
@@ -2798,7 +2834,7 @@
       <c r="X8" s="54"/>
       <c r="Y8" s="19"/>
     </row>
-    <row r="9" spans="1:25" s="18" customFormat="1">
+    <row r="9" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="22"/>
@@ -2820,7 +2856,7 @@
       <c r="X9" s="54"/>
       <c r="Y9" s="19"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="18"/>
       <c r="C10" s="26"/>
@@ -2842,7 +2878,7 @@
       <c r="X10" s="55"/>
       <c r="Y10" s="26"/>
     </row>
-    <row r="11" spans="1:25" s="10" customFormat="1">
+    <row r="11" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="D11" s="33"/>
@@ -2865,7 +2901,7 @@
       <c r="X11" s="56"/>
       <c r="Y11" s="16"/>
     </row>
-    <row r="12" spans="1:25" s="30" customFormat="1">
+    <row r="12" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="34"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -2889,7 +2925,7 @@
       <c r="X12" s="57"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="1:25" s="30" customFormat="1">
+    <row r="13" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="34"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -2910,7 +2946,7 @@
       <c r="X13" s="57"/>
       <c r="Y13" s="15"/>
     </row>
-    <row r="14" spans="1:25" s="30" customFormat="1">
+    <row r="14" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="34"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -2931,7 +2967,7 @@
       <c r="X14" s="57"/>
       <c r="Y14" s="15"/>
     </row>
-    <row r="15" spans="1:25" s="30" customFormat="1">
+    <row r="15" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="34"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -2952,7 +2988,7 @@
       <c r="X15" s="57"/>
       <c r="Y15" s="15"/>
     </row>
-    <row r="16" spans="1:25" s="30" customFormat="1">
+    <row r="16" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="34"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -2973,7 +3009,7 @@
       <c r="X16" s="57"/>
       <c r="Y16" s="15"/>
     </row>
-    <row r="17" spans="4:25" s="30" customFormat="1">
+    <row r="17" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="34"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -2994,7 +3030,7 @@
       <c r="X17" s="57"/>
       <c r="Y17" s="15"/>
     </row>
-    <row r="18" spans="4:25" s="30" customFormat="1">
+    <row r="18" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="34"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -3015,7 +3051,7 @@
       <c r="X18" s="57"/>
       <c r="Y18" s="15"/>
     </row>
-    <row r="19" spans="4:25" s="30" customFormat="1">
+    <row r="19" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="34"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -3036,7 +3072,7 @@
       <c r="X19" s="57"/>
       <c r="Y19" s="15"/>
     </row>
-    <row r="20" spans="4:25" s="30" customFormat="1">
+    <row r="20" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="34"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -3057,7 +3093,7 @@
       <c r="X20" s="57"/>
       <c r="Y20" s="15"/>
     </row>
-    <row r="21" spans="4:25" s="30" customFormat="1">
+    <row r="21" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="34"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -3078,7 +3114,7 @@
       <c r="X21" s="57"/>
       <c r="Y21" s="15"/>
     </row>
-    <row r="22" spans="4:25" s="30" customFormat="1">
+    <row r="22" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="34"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -3099,7 +3135,7 @@
       <c r="X22" s="57"/>
       <c r="Y22" s="15"/>
     </row>
-    <row r="23" spans="4:25" s="30" customFormat="1">
+    <row r="23" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="34"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -3120,7 +3156,7 @@
       <c r="X23" s="57"/>
       <c r="Y23" s="15"/>
     </row>
-    <row r="24" spans="4:25" s="30" customFormat="1">
+    <row r="24" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="34"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -3141,7 +3177,7 @@
       <c r="X24" s="57"/>
       <c r="Y24" s="15"/>
     </row>
-    <row r="25" spans="4:25" s="30" customFormat="1">
+    <row r="25" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="34"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -3162,7 +3198,7 @@
       <c r="X25" s="57"/>
       <c r="Y25" s="15"/>
     </row>
-    <row r="26" spans="4:25" s="30" customFormat="1">
+    <row r="26" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="34"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -3183,7 +3219,7 @@
       <c r="X26" s="57"/>
       <c r="Y26" s="15"/>
     </row>
-    <row r="27" spans="4:25" s="30" customFormat="1">
+    <row r="27" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="34"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -3204,7 +3240,7 @@
       <c r="X27" s="57"/>
       <c r="Y27" s="15"/>
     </row>
-    <row r="28" spans="4:25" s="30" customFormat="1">
+    <row r="28" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="34"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -3225,7 +3261,7 @@
       <c r="X28" s="57"/>
       <c r="Y28" s="15"/>
     </row>
-    <row r="29" spans="4:25" s="30" customFormat="1">
+    <row r="29" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="34"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -3246,7 +3282,7 @@
       <c r="X29" s="57"/>
       <c r="Y29" s="15"/>
     </row>
-    <row r="30" spans="4:25" s="30" customFormat="1">
+    <row r="30" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="34"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -3280,117 +3316,117 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" style="13" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="12"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
     </row>
   </sheetData>
@@ -3402,11 +3438,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="60" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="45" bestFit="1" customWidth="1"/>
@@ -3415,13 +3451,13 @@
     <col min="5" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="64" customFormat="1" ht="16.5" customHeight="1">
+    <row r="1" spans="1:4" s="64" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="63" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" customHeight="1"/>
-    <row r="3" spans="1:4" s="65" customFormat="1" ht="16.5" customHeight="1">
+    <row r="2" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:4" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
         <v>4</v>
       </c>
@@ -3435,7 +3471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="60">
         <v>1</v>
       </c>
@@ -3449,9 +3485,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="62">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="59" t="s">
         <v>12</v>
@@ -3461,6 +3497,34 @@
       </c>
       <c r="D5" s="61">
         <v>43282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3476,22 +3540,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="50.7109375" style="7" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="58"/>
     </row>
@@ -3509,7 +3573,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="13" customWidth="1"/>
@@ -3537,11 +3601,11 @@
     <col min="28" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
     </row>
-    <row r="3" spans="1:27" s="18" customFormat="1">
+    <row r="3" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="23"/>
       <c r="D3" s="21"/>
       <c r="K3" s="47"/>
@@ -3562,7 +3626,7 @@
       <c r="Z3" s="54"/>
       <c r="AA3" s="19"/>
     </row>
-    <row r="4" spans="1:27" s="18" customFormat="1">
+    <row r="4" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="23"/>
       <c r="D4" s="21"/>
       <c r="K4" s="47"/>
@@ -3583,7 +3647,7 @@
       <c r="Z4" s="54"/>
       <c r="AA4" s="19"/>
     </row>
-    <row r="5" spans="1:27" s="18" customFormat="1">
+    <row r="5" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="23"/>
       <c r="D5" s="21"/>
       <c r="K5" s="47"/>
@@ -3604,7 +3668,7 @@
       <c r="Z5" s="54"/>
       <c r="AA5" s="19"/>
     </row>
-    <row r="6" spans="1:27" s="18" customFormat="1">
+    <row r="6" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="21"/>
       <c r="K6" s="47"/>
       <c r="L6" s="51"/>
@@ -3624,7 +3688,7 @@
       <c r="Z6" s="54"/>
       <c r="AA6" s="19"/>
     </row>
-    <row r="7" spans="1:27" s="18" customFormat="1">
+    <row r="7" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="D7" s="21"/>
       <c r="F7" s="19"/>
@@ -3646,7 +3710,7 @@
       <c r="Z7" s="54"/>
       <c r="AA7" s="19"/>
     </row>
-    <row r="8" spans="1:27" s="18" customFormat="1">
+    <row r="8" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="22"/>
@@ -3669,7 +3733,7 @@
       <c r="Z8" s="54"/>
       <c r="AA8" s="19"/>
     </row>
-    <row r="9" spans="1:27" s="18" customFormat="1">
+    <row r="9" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="22"/>
@@ -3692,7 +3756,7 @@
       <c r="Z9" s="54"/>
       <c r="AA9" s="19"/>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="18"/>
       <c r="C10" s="26"/>
@@ -3714,7 +3778,7 @@
       <c r="Z10" s="55"/>
       <c r="AA10" s="26"/>
     </row>
-    <row r="11" spans="1:27" s="10" customFormat="1">
+    <row r="11" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="D11" s="33"/>
@@ -3738,7 +3802,7 @@
       <c r="Z11" s="56"/>
       <c r="AA11" s="16"/>
     </row>
-    <row r="12" spans="1:27" s="30" customFormat="1">
+    <row r="12" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="34"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -3763,7 +3827,7 @@
       <c r="Z12" s="57"/>
       <c r="AA12" s="15"/>
     </row>
-    <row r="13" spans="1:27" s="30" customFormat="1">
+    <row r="13" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="34"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -3785,7 +3849,7 @@
       <c r="Z13" s="57"/>
       <c r="AA13" s="15"/>
     </row>
-    <row r="14" spans="1:27" s="30" customFormat="1">
+    <row r="14" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="34"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -3807,7 +3871,7 @@
       <c r="Z14" s="57"/>
       <c r="AA14" s="15"/>
     </row>
-    <row r="15" spans="1:27" s="30" customFormat="1">
+    <row r="15" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="34"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -3829,7 +3893,7 @@
       <c r="Z15" s="57"/>
       <c r="AA15" s="15"/>
     </row>
-    <row r="16" spans="1:27" s="30" customFormat="1">
+    <row r="16" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="34"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -3851,7 +3915,7 @@
       <c r="Z16" s="57"/>
       <c r="AA16" s="15"/>
     </row>
-    <row r="17" spans="4:27" s="30" customFormat="1">
+    <row r="17" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="34"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -3873,7 +3937,7 @@
       <c r="Z17" s="57"/>
       <c r="AA17" s="15"/>
     </row>
-    <row r="18" spans="4:27" s="30" customFormat="1">
+    <row r="18" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="34"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -3895,7 +3959,7 @@
       <c r="Z18" s="57"/>
       <c r="AA18" s="15"/>
     </row>
-    <row r="19" spans="4:27" s="30" customFormat="1">
+    <row r="19" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="34"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -3917,7 +3981,7 @@
       <c r="Z19" s="57"/>
       <c r="AA19" s="15"/>
     </row>
-    <row r="20" spans="4:27" s="30" customFormat="1">
+    <row r="20" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="34"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -3939,7 +4003,7 @@
       <c r="Z20" s="57"/>
       <c r="AA20" s="15"/>
     </row>
-    <row r="21" spans="4:27" s="30" customFormat="1">
+    <row r="21" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="34"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -3961,7 +4025,7 @@
       <c r="Z21" s="57"/>
       <c r="AA21" s="15"/>
     </row>
-    <row r="22" spans="4:27" s="30" customFormat="1">
+    <row r="22" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="34"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -3983,7 +4047,7 @@
       <c r="Z22" s="57"/>
       <c r="AA22" s="15"/>
     </row>
-    <row r="23" spans="4:27" s="30" customFormat="1">
+    <row r="23" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="34"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -4005,7 +4069,7 @@
       <c r="Z23" s="57"/>
       <c r="AA23" s="15"/>
     </row>
-    <row r="24" spans="4:27" s="30" customFormat="1">
+    <row r="24" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="34"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -4027,7 +4091,7 @@
       <c r="Z24" s="57"/>
       <c r="AA24" s="15"/>
     </row>
-    <row r="25" spans="4:27" s="30" customFormat="1">
+    <row r="25" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="34"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -4049,7 +4113,7 @@
       <c r="Z25" s="57"/>
       <c r="AA25" s="15"/>
     </row>
-    <row r="26" spans="4:27" s="30" customFormat="1">
+    <row r="26" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="34"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -4071,7 +4135,7 @@
       <c r="Z26" s="57"/>
       <c r="AA26" s="15"/>
     </row>
-    <row r="27" spans="4:27" s="30" customFormat="1">
+    <row r="27" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="34"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -4093,7 +4157,7 @@
       <c r="Z27" s="57"/>
       <c r="AA27" s="15"/>
     </row>
-    <row r="28" spans="4:27" s="30" customFormat="1">
+    <row r="28" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="34"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -4115,7 +4179,7 @@
       <c r="Z28" s="57"/>
       <c r="AA28" s="15"/>
     </row>
-    <row r="29" spans="4:27" s="30" customFormat="1">
+    <row r="29" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="34"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -4137,7 +4201,7 @@
       <c r="Z29" s="57"/>
       <c r="AA29" s="15"/>
     </row>
-    <row r="30" spans="4:27" s="30" customFormat="1">
+    <row r="30" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="34"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -4172,7 +4236,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="13" customWidth="1"/>
@@ -4200,11 +4264,11 @@
     <col min="28" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
     </row>
-    <row r="3" spans="1:27" s="18" customFormat="1">
+    <row r="3" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="23"/>
       <c r="D3" s="21"/>
       <c r="K3" s="47"/>
@@ -4225,7 +4289,7 @@
       <c r="Z3" s="54"/>
       <c r="AA3" s="19"/>
     </row>
-    <row r="4" spans="1:27" s="18" customFormat="1">
+    <row r="4" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="23"/>
       <c r="D4" s="21"/>
       <c r="K4" s="47"/>
@@ -4246,7 +4310,7 @@
       <c r="Z4" s="54"/>
       <c r="AA4" s="19"/>
     </row>
-    <row r="5" spans="1:27" s="18" customFormat="1">
+    <row r="5" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="23"/>
       <c r="D5" s="21"/>
       <c r="K5" s="47"/>
@@ -4267,7 +4331,7 @@
       <c r="Z5" s="54"/>
       <c r="AA5" s="19"/>
     </row>
-    <row r="6" spans="1:27" s="18" customFormat="1">
+    <row r="6" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="21"/>
       <c r="K6" s="47"/>
       <c r="L6" s="51"/>
@@ -4287,7 +4351,7 @@
       <c r="Z6" s="54"/>
       <c r="AA6" s="19"/>
     </row>
-    <row r="7" spans="1:27" s="18" customFormat="1">
+    <row r="7" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="D7" s="21"/>
       <c r="F7" s="19"/>
@@ -4309,7 +4373,7 @@
       <c r="Z7" s="54"/>
       <c r="AA7" s="19"/>
     </row>
-    <row r="8" spans="1:27" s="18" customFormat="1">
+    <row r="8" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="22"/>
@@ -4332,7 +4396,7 @@
       <c r="Z8" s="54"/>
       <c r="AA8" s="19"/>
     </row>
-    <row r="9" spans="1:27" s="18" customFormat="1">
+    <row r="9" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="22"/>
@@ -4355,7 +4419,7 @@
       <c r="Z9" s="54"/>
       <c r="AA9" s="19"/>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="18"/>
       <c r="C10" s="26"/>
@@ -4377,7 +4441,7 @@
       <c r="Z10" s="55"/>
       <c r="AA10" s="26"/>
     </row>
-    <row r="11" spans="1:27" s="10" customFormat="1">
+    <row r="11" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="D11" s="33"/>
@@ -4401,7 +4465,7 @@
       <c r="Z11" s="56"/>
       <c r="AA11" s="16"/>
     </row>
-    <row r="12" spans="1:27" s="30" customFormat="1">
+    <row r="12" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="34"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -4426,7 +4490,7 @@
       <c r="Z12" s="57"/>
       <c r="AA12" s="15"/>
     </row>
-    <row r="13" spans="1:27" s="30" customFormat="1">
+    <row r="13" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="34"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -4448,7 +4512,7 @@
       <c r="Z13" s="57"/>
       <c r="AA13" s="15"/>
     </row>
-    <row r="14" spans="1:27" s="30" customFormat="1">
+    <row r="14" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="34"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -4470,7 +4534,7 @@
       <c r="Z14" s="57"/>
       <c r="AA14" s="15"/>
     </row>
-    <row r="15" spans="1:27" s="30" customFormat="1">
+    <row r="15" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="34"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -4492,7 +4556,7 @@
       <c r="Z15" s="57"/>
       <c r="AA15" s="15"/>
     </row>
-    <row r="16" spans="1:27" s="30" customFormat="1">
+    <row r="16" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="34"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -4514,7 +4578,7 @@
       <c r="Z16" s="57"/>
       <c r="AA16" s="15"/>
     </row>
-    <row r="17" spans="4:27" s="30" customFormat="1">
+    <row r="17" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="34"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -4536,7 +4600,7 @@
       <c r="Z17" s="57"/>
       <c r="AA17" s="15"/>
     </row>
-    <row r="18" spans="4:27" s="30" customFormat="1">
+    <row r="18" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="34"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -4558,7 +4622,7 @@
       <c r="Z18" s="57"/>
       <c r="AA18" s="15"/>
     </row>
-    <row r="19" spans="4:27" s="30" customFormat="1">
+    <row r="19" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="34"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -4580,7 +4644,7 @@
       <c r="Z19" s="57"/>
       <c r="AA19" s="15"/>
     </row>
-    <row r="20" spans="4:27" s="30" customFormat="1">
+    <row r="20" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="34"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -4602,7 +4666,7 @@
       <c r="Z20" s="57"/>
       <c r="AA20" s="15"/>
     </row>
-    <row r="21" spans="4:27" s="30" customFormat="1">
+    <row r="21" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="34"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -4624,7 +4688,7 @@
       <c r="Z21" s="57"/>
       <c r="AA21" s="15"/>
     </row>
-    <row r="22" spans="4:27" s="30" customFormat="1">
+    <row r="22" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="34"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -4646,7 +4710,7 @@
       <c r="Z22" s="57"/>
       <c r="AA22" s="15"/>
     </row>
-    <row r="23" spans="4:27" s="30" customFormat="1">
+    <row r="23" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="34"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -4668,7 +4732,7 @@
       <c r="Z23" s="57"/>
       <c r="AA23" s="15"/>
     </row>
-    <row r="24" spans="4:27" s="30" customFormat="1">
+    <row r="24" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="34"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -4690,7 +4754,7 @@
       <c r="Z24" s="57"/>
       <c r="AA24" s="15"/>
     </row>
-    <row r="25" spans="4:27" s="30" customFormat="1">
+    <row r="25" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="34"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -4712,7 +4776,7 @@
       <c r="Z25" s="57"/>
       <c r="AA25" s="15"/>
     </row>
-    <row r="26" spans="4:27" s="30" customFormat="1">
+    <row r="26" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="34"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -4734,7 +4798,7 @@
       <c r="Z26" s="57"/>
       <c r="AA26" s="15"/>
     </row>
-    <row r="27" spans="4:27" s="30" customFormat="1">
+    <row r="27" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="34"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -4756,7 +4820,7 @@
       <c r="Z27" s="57"/>
       <c r="AA27" s="15"/>
     </row>
-    <row r="28" spans="4:27" s="30" customFormat="1">
+    <row r="28" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="34"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -4778,7 +4842,7 @@
       <c r="Z28" s="57"/>
       <c r="AA28" s="15"/>
     </row>
-    <row r="29" spans="4:27" s="30" customFormat="1">
+    <row r="29" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="34"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -4800,7 +4864,7 @@
       <c r="Z29" s="57"/>
       <c r="AA29" s="15"/>
     </row>
-    <row r="30" spans="4:27" s="30" customFormat="1">
+    <row r="30" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="34"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -4835,7 +4899,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="13" customWidth="1"/>
@@ -4863,11 +4927,11 @@
     <col min="28" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
     </row>
-    <row r="3" spans="1:27" s="18" customFormat="1">
+    <row r="3" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="23"/>
       <c r="D3" s="21"/>
       <c r="K3" s="47"/>
@@ -4888,7 +4952,7 @@
       <c r="Z3" s="54"/>
       <c r="AA3" s="19"/>
     </row>
-    <row r="4" spans="1:27" s="18" customFormat="1">
+    <row r="4" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="23"/>
       <c r="D4" s="21"/>
       <c r="K4" s="47"/>
@@ -4909,7 +4973,7 @@
       <c r="Z4" s="54"/>
       <c r="AA4" s="19"/>
     </row>
-    <row r="5" spans="1:27" s="18" customFormat="1">
+    <row r="5" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="23"/>
       <c r="D5" s="21"/>
       <c r="K5" s="47"/>
@@ -4930,7 +4994,7 @@
       <c r="Z5" s="54"/>
       <c r="AA5" s="19"/>
     </row>
-    <row r="6" spans="1:27" s="18" customFormat="1">
+    <row r="6" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="21"/>
       <c r="K6" s="47"/>
       <c r="L6" s="51"/>
@@ -4950,7 +5014,7 @@
       <c r="Z6" s="54"/>
       <c r="AA6" s="19"/>
     </row>
-    <row r="7" spans="1:27" s="18" customFormat="1">
+    <row r="7" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="D7" s="21"/>
       <c r="F7" s="19"/>
@@ -4972,7 +5036,7 @@
       <c r="Z7" s="54"/>
       <c r="AA7" s="19"/>
     </row>
-    <row r="8" spans="1:27" s="18" customFormat="1">
+    <row r="8" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="22"/>
@@ -4995,7 +5059,7 @@
       <c r="Z8" s="54"/>
       <c r="AA8" s="19"/>
     </row>
-    <row r="9" spans="1:27" s="18" customFormat="1">
+    <row r="9" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="22"/>
@@ -5018,7 +5082,7 @@
       <c r="Z9" s="54"/>
       <c r="AA9" s="19"/>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="18"/>
       <c r="C10" s="26"/>
@@ -5040,7 +5104,7 @@
       <c r="Z10" s="55"/>
       <c r="AA10" s="26"/>
     </row>
-    <row r="11" spans="1:27" s="10" customFormat="1">
+    <row r="11" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="D11" s="33"/>
@@ -5064,7 +5128,7 @@
       <c r="Z11" s="56"/>
       <c r="AA11" s="16"/>
     </row>
-    <row r="12" spans="1:27" s="30" customFormat="1">
+    <row r="12" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="34"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -5089,7 +5153,7 @@
       <c r="Z12" s="57"/>
       <c r="AA12" s="15"/>
     </row>
-    <row r="13" spans="1:27" s="30" customFormat="1">
+    <row r="13" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="34"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -5111,7 +5175,7 @@
       <c r="Z13" s="57"/>
       <c r="AA13" s="15"/>
     </row>
-    <row r="14" spans="1:27" s="30" customFormat="1">
+    <row r="14" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="34"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -5133,7 +5197,7 @@
       <c r="Z14" s="57"/>
       <c r="AA14" s="15"/>
     </row>
-    <row r="15" spans="1:27" s="30" customFormat="1">
+    <row r="15" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="34"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -5155,7 +5219,7 @@
       <c r="Z15" s="57"/>
       <c r="AA15" s="15"/>
     </row>
-    <row r="16" spans="1:27" s="30" customFormat="1">
+    <row r="16" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="34"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -5177,7 +5241,7 @@
       <c r="Z16" s="57"/>
       <c r="AA16" s="15"/>
     </row>
-    <row r="17" spans="4:27" s="30" customFormat="1">
+    <row r="17" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="34"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -5199,7 +5263,7 @@
       <c r="Z17" s="57"/>
       <c r="AA17" s="15"/>
     </row>
-    <row r="18" spans="4:27" s="30" customFormat="1">
+    <row r="18" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="34"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -5221,7 +5285,7 @@
       <c r="Z18" s="57"/>
       <c r="AA18" s="15"/>
     </row>
-    <row r="19" spans="4:27" s="30" customFormat="1">
+    <row r="19" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="34"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -5243,7 +5307,7 @@
       <c r="Z19" s="57"/>
       <c r="AA19" s="15"/>
     </row>
-    <row r="20" spans="4:27" s="30" customFormat="1">
+    <row r="20" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="34"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -5265,7 +5329,7 @@
       <c r="Z20" s="57"/>
       <c r="AA20" s="15"/>
     </row>
-    <row r="21" spans="4:27" s="30" customFormat="1">
+    <row r="21" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="34"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -5287,7 +5351,7 @@
       <c r="Z21" s="57"/>
       <c r="AA21" s="15"/>
     </row>
-    <row r="22" spans="4:27" s="30" customFormat="1">
+    <row r="22" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="34"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -5309,7 +5373,7 @@
       <c r="Z22" s="57"/>
       <c r="AA22" s="15"/>
     </row>
-    <row r="23" spans="4:27" s="30" customFormat="1">
+    <row r="23" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="34"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -5331,7 +5395,7 @@
       <c r="Z23" s="57"/>
       <c r="AA23" s="15"/>
     </row>
-    <row r="24" spans="4:27" s="30" customFormat="1">
+    <row r="24" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="34"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -5353,7 +5417,7 @@
       <c r="Z24" s="57"/>
       <c r="AA24" s="15"/>
     </row>
-    <row r="25" spans="4:27" s="30" customFormat="1">
+    <row r="25" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="34"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -5375,7 +5439,7 @@
       <c r="Z25" s="57"/>
       <c r="AA25" s="15"/>
     </row>
-    <row r="26" spans="4:27" s="30" customFormat="1">
+    <row r="26" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="34"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -5397,7 +5461,7 @@
       <c r="Z26" s="57"/>
       <c r="AA26" s="15"/>
     </row>
-    <row r="27" spans="4:27" s="30" customFormat="1">
+    <row r="27" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="34"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -5419,7 +5483,7 @@
       <c r="Z27" s="57"/>
       <c r="AA27" s="15"/>
     </row>
-    <row r="28" spans="4:27" s="30" customFormat="1">
+    <row r="28" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="34"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -5441,7 +5505,7 @@
       <c r="Z28" s="57"/>
       <c r="AA28" s="15"/>
     </row>
-    <row r="29" spans="4:27" s="30" customFormat="1">
+    <row r="29" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="34"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -5463,7 +5527,7 @@
       <c r="Z29" s="57"/>
       <c r="AA29" s="15"/>
     </row>
-    <row r="30" spans="4:27" s="30" customFormat="1">
+    <row r="30" spans="4:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="34"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -5498,7 +5562,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="13" customWidth="1"/>
@@ -5524,11 +5588,11 @@
     <col min="26" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
     </row>
-    <row r="3" spans="1:25" s="18" customFormat="1">
+    <row r="3" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="23"/>
       <c r="D3" s="21"/>
       <c r="J3" s="51"/>
@@ -5548,7 +5612,7 @@
       <c r="X3" s="54"/>
       <c r="Y3" s="19"/>
     </row>
-    <row r="4" spans="1:25" s="18" customFormat="1">
+    <row r="4" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="23"/>
       <c r="D4" s="21"/>
       <c r="J4" s="51"/>
@@ -5568,7 +5632,7 @@
       <c r="X4" s="54"/>
       <c r="Y4" s="19"/>
     </row>
-    <row r="5" spans="1:25" s="18" customFormat="1">
+    <row r="5" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="23"/>
       <c r="D5" s="21"/>
       <c r="J5" s="51"/>
@@ -5588,7 +5652,7 @@
       <c r="X5" s="54"/>
       <c r="Y5" s="19"/>
     </row>
-    <row r="6" spans="1:25" s="18" customFormat="1">
+    <row r="6" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="21"/>
       <c r="J6" s="51"/>
       <c r="K6" s="19"/>
@@ -5607,7 +5671,7 @@
       <c r="X6" s="54"/>
       <c r="Y6" s="19"/>
     </row>
-    <row r="7" spans="1:25" s="18" customFormat="1">
+    <row r="7" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="D7" s="21"/>
       <c r="F7" s="19"/>
@@ -5628,7 +5692,7 @@
       <c r="X7" s="54"/>
       <c r="Y7" s="19"/>
     </row>
-    <row r="8" spans="1:25" s="18" customFormat="1">
+    <row r="8" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="22"/>
@@ -5650,7 +5714,7 @@
       <c r="X8" s="54"/>
       <c r="Y8" s="19"/>
     </row>
-    <row r="9" spans="1:25" s="18" customFormat="1">
+    <row r="9" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="22"/>
@@ -5672,7 +5736,7 @@
       <c r="X9" s="54"/>
       <c r="Y9" s="19"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="18"/>
       <c r="C10" s="26"/>
@@ -5694,7 +5758,7 @@
       <c r="X10" s="55"/>
       <c r="Y10" s="26"/>
     </row>
-    <row r="11" spans="1:25" s="10" customFormat="1">
+    <row r="11" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="D11" s="33"/>
@@ -5717,7 +5781,7 @@
       <c r="X11" s="56"/>
       <c r="Y11" s="16"/>
     </row>
-    <row r="12" spans="1:25" s="30" customFormat="1">
+    <row r="12" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="34"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -5741,7 +5805,7 @@
       <c r="X12" s="57"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="1:25" s="30" customFormat="1">
+    <row r="13" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="34"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -5762,7 +5826,7 @@
       <c r="X13" s="57"/>
       <c r="Y13" s="15"/>
     </row>
-    <row r="14" spans="1:25" s="30" customFormat="1">
+    <row r="14" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="34"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -5783,7 +5847,7 @@
       <c r="X14" s="57"/>
       <c r="Y14" s="15"/>
     </row>
-    <row r="15" spans="1:25" s="30" customFormat="1">
+    <row r="15" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="34"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -5804,7 +5868,7 @@
       <c r="X15" s="57"/>
       <c r="Y15" s="15"/>
     </row>
-    <row r="16" spans="1:25" s="30" customFormat="1">
+    <row r="16" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="34"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -5825,7 +5889,7 @@
       <c r="X16" s="57"/>
       <c r="Y16" s="15"/>
     </row>
-    <row r="17" spans="4:25" s="30" customFormat="1">
+    <row r="17" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="34"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -5846,7 +5910,7 @@
       <c r="X17" s="57"/>
       <c r="Y17" s="15"/>
     </row>
-    <row r="18" spans="4:25" s="30" customFormat="1">
+    <row r="18" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="34"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -5867,7 +5931,7 @@
       <c r="X18" s="57"/>
       <c r="Y18" s="15"/>
     </row>
-    <row r="19" spans="4:25" s="30" customFormat="1">
+    <row r="19" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="34"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -5888,7 +5952,7 @@
       <c r="X19" s="57"/>
       <c r="Y19" s="15"/>
     </row>
-    <row r="20" spans="4:25" s="30" customFormat="1">
+    <row r="20" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="34"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -5909,7 +5973,7 @@
       <c r="X20" s="57"/>
       <c r="Y20" s="15"/>
     </row>
-    <row r="21" spans="4:25" s="30" customFormat="1">
+    <row r="21" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="34"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -5930,7 +5994,7 @@
       <c r="X21" s="57"/>
       <c r="Y21" s="15"/>
     </row>
-    <row r="22" spans="4:25" s="30" customFormat="1">
+    <row r="22" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="34"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -5951,7 +6015,7 @@
       <c r="X22" s="57"/>
       <c r="Y22" s="15"/>
     </row>
-    <row r="23" spans="4:25" s="30" customFormat="1">
+    <row r="23" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="34"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -5972,7 +6036,7 @@
       <c r="X23" s="57"/>
       <c r="Y23" s="15"/>
     </row>
-    <row r="24" spans="4:25" s="30" customFormat="1">
+    <row r="24" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="34"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -5993,7 +6057,7 @@
       <c r="X24" s="57"/>
       <c r="Y24" s="15"/>
     </row>
-    <row r="25" spans="4:25" s="30" customFormat="1">
+    <row r="25" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="34"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -6014,7 +6078,7 @@
       <c r="X25" s="57"/>
       <c r="Y25" s="15"/>
     </row>
-    <row r="26" spans="4:25" s="30" customFormat="1">
+    <row r="26" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="34"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -6035,7 +6099,7 @@
       <c r="X26" s="57"/>
       <c r="Y26" s="15"/>
     </row>
-    <row r="27" spans="4:25" s="30" customFormat="1">
+    <row r="27" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="34"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -6056,7 +6120,7 @@
       <c r="X27" s="57"/>
       <c r="Y27" s="15"/>
     </row>
-    <row r="28" spans="4:25" s="30" customFormat="1">
+    <row r="28" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="34"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -6077,7 +6141,7 @@
       <c r="X28" s="57"/>
       <c r="Y28" s="15"/>
     </row>
-    <row r="29" spans="4:25" s="30" customFormat="1">
+    <row r="29" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="34"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -6098,7 +6162,7 @@
       <c r="X29" s="57"/>
       <c r="Y29" s="15"/>
     </row>
-    <row r="30" spans="4:25" s="30" customFormat="1">
+    <row r="30" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="34"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -6132,7 +6196,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="13" customWidth="1"/>
@@ -6158,11 +6222,11 @@
     <col min="26" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
     </row>
-    <row r="3" spans="1:25" s="18" customFormat="1">
+    <row r="3" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="23"/>
       <c r="D3" s="21"/>
       <c r="J3" s="51"/>
@@ -6182,7 +6246,7 @@
       <c r="X3" s="54"/>
       <c r="Y3" s="19"/>
     </row>
-    <row r="4" spans="1:25" s="18" customFormat="1">
+    <row r="4" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="23"/>
       <c r="D4" s="21"/>
       <c r="J4" s="51"/>
@@ -6202,7 +6266,7 @@
       <c r="X4" s="54"/>
       <c r="Y4" s="19"/>
     </row>
-    <row r="5" spans="1:25" s="18" customFormat="1">
+    <row r="5" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="23"/>
       <c r="D5" s="21"/>
       <c r="J5" s="51"/>
@@ -6222,7 +6286,7 @@
       <c r="X5" s="54"/>
       <c r="Y5" s="19"/>
     </row>
-    <row r="6" spans="1:25" s="18" customFormat="1">
+    <row r="6" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="21"/>
       <c r="J6" s="51"/>
       <c r="K6" s="19"/>
@@ -6241,7 +6305,7 @@
       <c r="X6" s="54"/>
       <c r="Y6" s="19"/>
     </row>
-    <row r="7" spans="1:25" s="18" customFormat="1">
+    <row r="7" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="D7" s="21"/>
       <c r="F7" s="19"/>
@@ -6262,7 +6326,7 @@
       <c r="X7" s="54"/>
       <c r="Y7" s="19"/>
     </row>
-    <row r="8" spans="1:25" s="18" customFormat="1">
+    <row r="8" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="22"/>
@@ -6284,7 +6348,7 @@
       <c r="X8" s="54"/>
       <c r="Y8" s="19"/>
     </row>
-    <row r="9" spans="1:25" s="18" customFormat="1">
+    <row r="9" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="22"/>
@@ -6306,7 +6370,7 @@
       <c r="X9" s="54"/>
       <c r="Y9" s="19"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="18"/>
       <c r="C10" s="26"/>
@@ -6328,7 +6392,7 @@
       <c r="X10" s="55"/>
       <c r="Y10" s="26"/>
     </row>
-    <row r="11" spans="1:25" s="10" customFormat="1">
+    <row r="11" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="D11" s="33"/>
@@ -6351,7 +6415,7 @@
       <c r="X11" s="56"/>
       <c r="Y11" s="16"/>
     </row>
-    <row r="12" spans="1:25" s="30" customFormat="1">
+    <row r="12" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="34"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -6375,7 +6439,7 @@
       <c r="X12" s="57"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="1:25" s="30" customFormat="1">
+    <row r="13" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="34"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -6396,7 +6460,7 @@
       <c r="X13" s="57"/>
       <c r="Y13" s="15"/>
     </row>
-    <row r="14" spans="1:25" s="30" customFormat="1">
+    <row r="14" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="34"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -6417,7 +6481,7 @@
       <c r="X14" s="57"/>
       <c r="Y14" s="15"/>
     </row>
-    <row r="15" spans="1:25" s="30" customFormat="1">
+    <row r="15" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="34"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -6438,7 +6502,7 @@
       <c r="X15" s="57"/>
       <c r="Y15" s="15"/>
     </row>
-    <row r="16" spans="1:25" s="30" customFormat="1">
+    <row r="16" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="34"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -6459,7 +6523,7 @@
       <c r="X16" s="57"/>
       <c r="Y16" s="15"/>
     </row>
-    <row r="17" spans="4:25" s="30" customFormat="1">
+    <row r="17" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="34"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -6480,7 +6544,7 @@
       <c r="X17" s="57"/>
       <c r="Y17" s="15"/>
     </row>
-    <row r="18" spans="4:25" s="30" customFormat="1">
+    <row r="18" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="34"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -6501,7 +6565,7 @@
       <c r="X18" s="57"/>
       <c r="Y18" s="15"/>
     </row>
-    <row r="19" spans="4:25" s="30" customFormat="1">
+    <row r="19" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="34"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -6522,7 +6586,7 @@
       <c r="X19" s="57"/>
       <c r="Y19" s="15"/>
     </row>
-    <row r="20" spans="4:25" s="30" customFormat="1">
+    <row r="20" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="34"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -6543,7 +6607,7 @@
       <c r="X20" s="57"/>
       <c r="Y20" s="15"/>
     </row>
-    <row r="21" spans="4:25" s="30" customFormat="1">
+    <row r="21" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="34"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -6564,7 +6628,7 @@
       <c r="X21" s="57"/>
       <c r="Y21" s="15"/>
     </row>
-    <row r="22" spans="4:25" s="30" customFormat="1">
+    <row r="22" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="34"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -6585,7 +6649,7 @@
       <c r="X22" s="57"/>
       <c r="Y22" s="15"/>
     </row>
-    <row r="23" spans="4:25" s="30" customFormat="1">
+    <row r="23" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="34"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -6606,7 +6670,7 @@
       <c r="X23" s="57"/>
       <c r="Y23" s="15"/>
     </row>
-    <row r="24" spans="4:25" s="30" customFormat="1">
+    <row r="24" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="34"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -6627,7 +6691,7 @@
       <c r="X24" s="57"/>
       <c r="Y24" s="15"/>
     </row>
-    <row r="25" spans="4:25" s="30" customFormat="1">
+    <row r="25" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="34"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -6648,7 +6712,7 @@
       <c r="X25" s="57"/>
       <c r="Y25" s="15"/>
     </row>
-    <row r="26" spans="4:25" s="30" customFormat="1">
+    <row r="26" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="34"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -6669,7 +6733,7 @@
       <c r="X26" s="57"/>
       <c r="Y26" s="15"/>
     </row>
-    <row r="27" spans="4:25" s="30" customFormat="1">
+    <row r="27" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="34"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -6690,7 +6754,7 @@
       <c r="X27" s="57"/>
       <c r="Y27" s="15"/>
     </row>
-    <row r="28" spans="4:25" s="30" customFormat="1">
+    <row r="28" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="34"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -6711,7 +6775,7 @@
       <c r="X28" s="57"/>
       <c r="Y28" s="15"/>
     </row>
-    <row r="29" spans="4:25" s="30" customFormat="1">
+    <row r="29" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="34"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -6732,7 +6796,7 @@
       <c r="X29" s="57"/>
       <c r="Y29" s="15"/>
     </row>
-    <row r="30" spans="4:25" s="30" customFormat="1">
+    <row r="30" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="34"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -6766,7 +6830,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="13" customWidth="1"/>
@@ -6792,11 +6856,11 @@
     <col min="26" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
     </row>
-    <row r="3" spans="1:25" s="18" customFormat="1">
+    <row r="3" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="23"/>
       <c r="D3" s="21"/>
       <c r="J3" s="51"/>
@@ -6816,7 +6880,7 @@
       <c r="X3" s="54"/>
       <c r="Y3" s="19"/>
     </row>
-    <row r="4" spans="1:25" s="18" customFormat="1">
+    <row r="4" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="23"/>
       <c r="D4" s="21"/>
       <c r="J4" s="51"/>
@@ -6836,7 +6900,7 @@
       <c r="X4" s="54"/>
       <c r="Y4" s="19"/>
     </row>
-    <row r="5" spans="1:25" s="18" customFormat="1">
+    <row r="5" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="23"/>
       <c r="D5" s="21"/>
       <c r="J5" s="51"/>
@@ -6856,7 +6920,7 @@
       <c r="X5" s="54"/>
       <c r="Y5" s="19"/>
     </row>
-    <row r="6" spans="1:25" s="18" customFormat="1">
+    <row r="6" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="21"/>
       <c r="J6" s="51"/>
       <c r="K6" s="19"/>
@@ -6875,7 +6939,7 @@
       <c r="X6" s="54"/>
       <c r="Y6" s="19"/>
     </row>
-    <row r="7" spans="1:25" s="18" customFormat="1">
+    <row r="7" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="D7" s="21"/>
       <c r="F7" s="19"/>
@@ -6896,7 +6960,7 @@
       <c r="X7" s="54"/>
       <c r="Y7" s="19"/>
     </row>
-    <row r="8" spans="1:25" s="18" customFormat="1">
+    <row r="8" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="22"/>
@@ -6918,7 +6982,7 @@
       <c r="X8" s="54"/>
       <c r="Y8" s="19"/>
     </row>
-    <row r="9" spans="1:25" s="18" customFormat="1">
+    <row r="9" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="22"/>
@@ -6940,7 +7004,7 @@
       <c r="X9" s="54"/>
       <c r="Y9" s="19"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="18"/>
       <c r="C10" s="26"/>
@@ -6962,7 +7026,7 @@
       <c r="X10" s="55"/>
       <c r="Y10" s="26"/>
     </row>
-    <row r="11" spans="1:25" s="10" customFormat="1">
+    <row r="11" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="D11" s="33"/>
@@ -6985,7 +7049,7 @@
       <c r="X11" s="56"/>
       <c r="Y11" s="16"/>
     </row>
-    <row r="12" spans="1:25" s="30" customFormat="1">
+    <row r="12" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="34"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -7009,7 +7073,7 @@
       <c r="X12" s="57"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="1:25" s="30" customFormat="1">
+    <row r="13" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="34"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -7030,7 +7094,7 @@
       <c r="X13" s="57"/>
       <c r="Y13" s="15"/>
     </row>
-    <row r="14" spans="1:25" s="30" customFormat="1">
+    <row r="14" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="34"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -7051,7 +7115,7 @@
       <c r="X14" s="57"/>
       <c r="Y14" s="15"/>
     </row>
-    <row r="15" spans="1:25" s="30" customFormat="1">
+    <row r="15" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="34"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -7072,7 +7136,7 @@
       <c r="X15" s="57"/>
       <c r="Y15" s="15"/>
     </row>
-    <row r="16" spans="1:25" s="30" customFormat="1">
+    <row r="16" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="34"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -7093,7 +7157,7 @@
       <c r="X16" s="57"/>
       <c r="Y16" s="15"/>
     </row>
-    <row r="17" spans="4:25" s="30" customFormat="1">
+    <row r="17" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="34"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -7114,7 +7178,7 @@
       <c r="X17" s="57"/>
       <c r="Y17" s="15"/>
     </row>
-    <row r="18" spans="4:25" s="30" customFormat="1">
+    <row r="18" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="34"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -7135,7 +7199,7 @@
       <c r="X18" s="57"/>
       <c r="Y18" s="15"/>
     </row>
-    <row r="19" spans="4:25" s="30" customFormat="1">
+    <row r="19" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="34"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -7156,7 +7220,7 @@
       <c r="X19" s="57"/>
       <c r="Y19" s="15"/>
     </row>
-    <row r="20" spans="4:25" s="30" customFormat="1">
+    <row r="20" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="34"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -7177,7 +7241,7 @@
       <c r="X20" s="57"/>
       <c r="Y20" s="15"/>
     </row>
-    <row r="21" spans="4:25" s="30" customFormat="1">
+    <row r="21" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="34"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -7198,7 +7262,7 @@
       <c r="X21" s="57"/>
       <c r="Y21" s="15"/>
     </row>
-    <row r="22" spans="4:25" s="30" customFormat="1">
+    <row r="22" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="34"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -7219,7 +7283,7 @@
       <c r="X22" s="57"/>
       <c r="Y22" s="15"/>
     </row>
-    <row r="23" spans="4:25" s="30" customFormat="1">
+    <row r="23" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="34"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -7240,7 +7304,7 @@
       <c r="X23" s="57"/>
       <c r="Y23" s="15"/>
     </row>
-    <row r="24" spans="4:25" s="30" customFormat="1">
+    <row r="24" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="34"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -7261,7 +7325,7 @@
       <c r="X24" s="57"/>
       <c r="Y24" s="15"/>
     </row>
-    <row r="25" spans="4:25" s="30" customFormat="1">
+    <row r="25" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="34"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -7282,7 +7346,7 @@
       <c r="X25" s="57"/>
       <c r="Y25" s="15"/>
     </row>
-    <row r="26" spans="4:25" s="30" customFormat="1">
+    <row r="26" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="34"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -7303,7 +7367,7 @@
       <c r="X26" s="57"/>
       <c r="Y26" s="15"/>
     </row>
-    <row r="27" spans="4:25" s="30" customFormat="1">
+    <row r="27" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="34"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -7324,7 +7388,7 @@
       <c r="X27" s="57"/>
       <c r="Y27" s="15"/>
     </row>
-    <row r="28" spans="4:25" s="30" customFormat="1">
+    <row r="28" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="34"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -7345,7 +7409,7 @@
       <c r="X28" s="57"/>
       <c r="Y28" s="15"/>
     </row>
-    <row r="29" spans="4:25" s="30" customFormat="1">
+    <row r="29" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="34"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -7366,7 +7430,7 @@
       <c r="X29" s="57"/>
       <c r="Y29" s="15"/>
     </row>
-    <row r="30" spans="4:25" s="30" customFormat="1">
+    <row r="30" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="34"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -7400,7 +7464,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="13" customWidth="1"/>
@@ -7426,11 +7490,11 @@
     <col min="26" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
     </row>
-    <row r="3" spans="1:25" s="18" customFormat="1">
+    <row r="3" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="23"/>
       <c r="D3" s="21"/>
       <c r="J3" s="51"/>
@@ -7450,7 +7514,7 @@
       <c r="X3" s="54"/>
       <c r="Y3" s="19"/>
     </row>
-    <row r="4" spans="1:25" s="18" customFormat="1">
+    <row r="4" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="23"/>
       <c r="D4" s="21"/>
       <c r="J4" s="51"/>
@@ -7470,7 +7534,7 @@
       <c r="X4" s="54"/>
       <c r="Y4" s="19"/>
     </row>
-    <row r="5" spans="1:25" s="18" customFormat="1">
+    <row r="5" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="23"/>
       <c r="D5" s="21"/>
       <c r="J5" s="51"/>
@@ -7490,7 +7554,7 @@
       <c r="X5" s="54"/>
       <c r="Y5" s="19"/>
     </row>
-    <row r="6" spans="1:25" s="18" customFormat="1">
+    <row r="6" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="21"/>
       <c r="J6" s="51"/>
       <c r="K6" s="19"/>
@@ -7509,7 +7573,7 @@
       <c r="X6" s="54"/>
       <c r="Y6" s="19"/>
     </row>
-    <row r="7" spans="1:25" s="18" customFormat="1">
+    <row r="7" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="D7" s="21"/>
       <c r="F7" s="19"/>
@@ -7530,7 +7594,7 @@
       <c r="X7" s="54"/>
       <c r="Y7" s="19"/>
     </row>
-    <row r="8" spans="1:25" s="18" customFormat="1">
+    <row r="8" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="22"/>
@@ -7552,7 +7616,7 @@
       <c r="X8" s="54"/>
       <c r="Y8" s="19"/>
     </row>
-    <row r="9" spans="1:25" s="18" customFormat="1">
+    <row r="9" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="22"/>
@@ -7574,7 +7638,7 @@
       <c r="X9" s="54"/>
       <c r="Y9" s="19"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="18"/>
       <c r="C10" s="26"/>
@@ -7596,7 +7660,7 @@
       <c r="X10" s="55"/>
       <c r="Y10" s="26"/>
     </row>
-    <row r="11" spans="1:25" s="10" customFormat="1">
+    <row r="11" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="D11" s="33"/>
@@ -7619,7 +7683,7 @@
       <c r="X11" s="56"/>
       <c r="Y11" s="16"/>
     </row>
-    <row r="12" spans="1:25" s="30" customFormat="1">
+    <row r="12" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="34"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -7643,7 +7707,7 @@
       <c r="X12" s="57"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="1:25" s="30" customFormat="1">
+    <row r="13" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="34"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -7664,7 +7728,7 @@
       <c r="X13" s="57"/>
       <c r="Y13" s="15"/>
     </row>
-    <row r="14" spans="1:25" s="30" customFormat="1">
+    <row r="14" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="34"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -7685,7 +7749,7 @@
       <c r="X14" s="57"/>
       <c r="Y14" s="15"/>
     </row>
-    <row r="15" spans="1:25" s="30" customFormat="1">
+    <row r="15" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="34"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -7706,7 +7770,7 @@
       <c r="X15" s="57"/>
       <c r="Y15" s="15"/>
     </row>
-    <row r="16" spans="1:25" s="30" customFormat="1">
+    <row r="16" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="34"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -7727,7 +7791,7 @@
       <c r="X16" s="57"/>
       <c r="Y16" s="15"/>
     </row>
-    <row r="17" spans="4:25" s="30" customFormat="1">
+    <row r="17" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="34"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -7748,7 +7812,7 @@
       <c r="X17" s="57"/>
       <c r="Y17" s="15"/>
     </row>
-    <row r="18" spans="4:25" s="30" customFormat="1">
+    <row r="18" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="34"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -7769,7 +7833,7 @@
       <c r="X18" s="57"/>
       <c r="Y18" s="15"/>
     </row>
-    <row r="19" spans="4:25" s="30" customFormat="1">
+    <row r="19" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="34"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -7790,7 +7854,7 @@
       <c r="X19" s="57"/>
       <c r="Y19" s="15"/>
     </row>
-    <row r="20" spans="4:25" s="30" customFormat="1">
+    <row r="20" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="34"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -7811,7 +7875,7 @@
       <c r="X20" s="57"/>
       <c r="Y20" s="15"/>
     </row>
-    <row r="21" spans="4:25" s="30" customFormat="1">
+    <row r="21" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="34"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -7832,7 +7896,7 @@
       <c r="X21" s="57"/>
       <c r="Y21" s="15"/>
     </row>
-    <row r="22" spans="4:25" s="30" customFormat="1">
+    <row r="22" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="34"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -7853,7 +7917,7 @@
       <c r="X22" s="57"/>
       <c r="Y22" s="15"/>
     </row>
-    <row r="23" spans="4:25" s="30" customFormat="1">
+    <row r="23" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="34"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -7874,7 +7938,7 @@
       <c r="X23" s="57"/>
       <c r="Y23" s="15"/>
     </row>
-    <row r="24" spans="4:25" s="30" customFormat="1">
+    <row r="24" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="34"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -7895,7 +7959,7 @@
       <c r="X24" s="57"/>
       <c r="Y24" s="15"/>
     </row>
-    <row r="25" spans="4:25" s="30" customFormat="1">
+    <row r="25" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="34"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -7916,7 +7980,7 @@
       <c r="X25" s="57"/>
       <c r="Y25" s="15"/>
     </row>
-    <row r="26" spans="4:25" s="30" customFormat="1">
+    <row r="26" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="34"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -7937,7 +8001,7 @@
       <c r="X26" s="57"/>
       <c r="Y26" s="15"/>
     </row>
-    <row r="27" spans="4:25" s="30" customFormat="1">
+    <row r="27" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="34"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -7958,7 +8022,7 @@
       <c r="X27" s="57"/>
       <c r="Y27" s="15"/>
     </row>
-    <row r="28" spans="4:25" s="30" customFormat="1">
+    <row r="28" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="34"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
@@ -7979,7 +8043,7 @@
       <c r="X28" s="57"/>
       <c r="Y28" s="15"/>
     </row>
-    <row r="29" spans="4:25" s="30" customFormat="1">
+    <row r="29" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="34"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -8000,7 +8064,7 @@
       <c r="X29" s="57"/>
       <c r="Y29" s="15"/>
     </row>
-    <row r="30" spans="4:25" s="30" customFormat="1">
+    <row r="30" spans="4:25" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="34"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>

</xml_diff>

<commit_message>
20210610 CRE21-006	Remove COVID19 bonus between VSS and RVP 20210610 CRE20-023-44	COVID-19 – Phase 44 	1.	Lower age limit to 12y 	2.	Block input remarks “\” and “|” 	3.	Revise outreach code C0001 – C0003 	4.	Add outreach list for school 	5.	Revise COVID19 Provider Name in eVacc interface 20210610 CRE21-004-02	To present the selected claim transactions in the Post Payment Check Reports (i.e. PPC0002 and PPC0003) in a randomized way – Phase 2 	1.	Any voucher schemes (HCVS, HCVSCHN, HCVSDHC) is selected in the criteria, the sorting order will be remained not randomized
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/PPC0002-Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/PPC0002-Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2021\CRE21-005 (Exclude C19 in PPC0002,PPC0003 and U0002)\Front-end\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2021\CRE21-004 (Randomise sorting of tx in PPC0002 and PPC0003)\Front-end (Phase 2)\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Description</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -118,6 +118,14 @@
   </si>
   <si>
     <t>2021/06/04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021/06/10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3438,7 +3446,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3525,6 +3533,20 @@
       </c>
       <c r="D7" s="60" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20210624 CRE21-004-03	To present the selected claim transactions in the Post Payment Check Reports (i.e. PPC0002 and PPC0003) in a randomized way – Phase 3
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/PPC0002-Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/PPC0002-Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2021\CRE21-004 (Randomise sorting of tx in PPC0002 and PPC0003)\Front-end (Phase 2)\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2021\CRE21-004 (Randomise sorting of tx in PPC0002 and PPC0003)\Front-end (Phase 3)\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Description</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -126,6 +126,14 @@
   </si>
   <si>
     <t>2021/06/10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021/06/24</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3446,7 +3454,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3547,6 +3555,20 @@
       </c>
       <c r="D8" s="60" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>